<commit_message>
Resonator packages filled in.
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@20312 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Resonators.xlsx
+++ b/Digikey/Resonators.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Stephen Deiss\Gadgetron\Gadgets\Libraries\Parts\Digikey\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="609" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="15825" tabRatio="609" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="5" r:id="rId1"/>
     <sheet name="SMD" sheetId="1" r:id="rId2"/>
     <sheet name="TH" sheetId="19" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="148">
   <si>
     <t>ï»¿"Datasheets"</t>
   </si>
@@ -456,6 +461,15 @@
   </si>
   <si>
     <t>V53-R0</t>
+  </si>
+  <si>
+    <t>MURATA_CTLS8_G_Series_HS</t>
+  </si>
+  <si>
+    <t>MURATA_CTLS8_X_Series_HS</t>
+  </si>
+  <si>
+    <t>MURATA_CSTCExxMyyV53-R0_HS</t>
   </si>
 </sst>
 </file>
@@ -716,13 +730,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -883,6 +900,16 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -965,18 +992,16 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -987,15 +1012,15 @@
     <sortCondition ref="A7:A44"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Target Value" dataDxfId="8"/>
-    <tableColumn id="11" name="Stock" dataDxfId="7"/>
-    <tableColumn id="6" name="Query" dataDxfId="6">
+    <tableColumn id="1" name="Target Value" dataDxfId="9"/>
+    <tableColumn id="11" name="Stock" dataDxfId="8"/>
+    <tableColumn id="6" name="Query" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE(Table4[[#This Row],[Target Value]],Table4[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="SMD" dataDxfId="5">
+    <tableColumn id="3" name="SMD" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],SMD!$AB$1:'SMD'!$AC$100,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="TH Status" dataDxfId="4">
+    <tableColumn id="4" name="TH Status" dataDxfId="5">
       <calculatedColumnFormula>VLOOKUP(Table4[[#This Row],[Query]],TH!$AB$1:'TH'!AD$300,1,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1041,11 +1066,11 @@
     <tableColumn id="23" name="Package / Case"/>
     <tableColumn id="25" name="Size / Dimension"/>
     <tableColumn id="26" name="Height"/>
-    <tableColumn id="30" name="Stock Freq?" dataDxfId="3">
+    <tableColumn id="30" name="Stock Freq?" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[Frequency]],Values!$A$11:'Values'!$D$20,2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="24" name="Stock"/>
-    <tableColumn id="27" name="Query" dataDxfId="2">
+    <tableColumn id="27" name="Query" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="28" name="Package"/>
@@ -1087,11 +1112,11 @@
     <tableColumn id="23" name="Package / Case"/>
     <tableColumn id="25" name="Size / Dimension"/>
     <tableColumn id="26" name="Height"/>
-    <tableColumn id="30" name="Stock Freq?" dataDxfId="1">
+    <tableColumn id="30" name="Stock Freq?" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table13[[#This Row],[Frequency]],Values!$A$11:'Values'!$D$20,2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="24" name="Stock"/>
-    <tableColumn id="27" name="Query" dataDxfId="0">
+    <tableColumn id="27" name="Query" dataDxfId="1">
       <calculatedColumnFormula>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="28" name="Package"/>
@@ -1429,20 +1454,20 @@
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -1450,7 +1475,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1458,10 +1483,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1478,7 +1503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1498,7 +1523,7 @@
         <v>10MHzStock</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1518,7 +1543,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1538,7 +1563,7 @@
         <v>16MHzStock</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1558,7 +1583,7 @@
         <v>20MHzStock</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1580,7 +1605,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D11:E15">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="STOCK">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="STOCK">
       <formula>NOT(ISERROR(SEARCH("STOCK",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1601,35 +1626,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="A1:AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="11" width="9.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="9.375" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="5" max="11" width="9.375" customWidth="1"/>
+    <col min="12" max="12" width="11.875" customWidth="1"/>
     <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.625" customWidth="1"/>
+    <col min="30" max="30" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16" thickBot="1">
+    <row r="1" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1748,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:30" hidden="1">
+    <row r="2" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1806,7 +1833,7 @@
         <v>10MHz</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="16" thickTop="1">
+    <row r="3" spans="1:30" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1893,11 +1920,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</f>
         <v>10MHzStock</v>
       </c>
+      <c r="AC3" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="AD3" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:30" hidden="1">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1982,7 +2012,7 @@
         <v>12MHz</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2069,11 +2099,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</f>
         <v>12MHzStock</v>
       </c>
+      <c r="AC5" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="AD5" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2160,11 +2193,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</f>
         <v>16MHzStock</v>
       </c>
+      <c r="AC6" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="AD6" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2251,11 +2287,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</f>
         <v>20MHzStock</v>
       </c>
+      <c r="AC7" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="AD7" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2342,11 +2381,14 @@
         <f>CONCATENATE(Table1[[#This Row],[Frequency]],Table1[[#This Row],[Stock]])</f>
         <v>8MHzStock</v>
       </c>
+      <c r="AC8" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="AD8" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:30" hidden="1">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2431,7 +2473,7 @@
         <v>8MHz</v>
       </c>
     </row>
-    <row r="10" spans="1:30" hidden="1">
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2516,7 +2558,7 @@
         <v>16MHz</v>
       </c>
     </row>
-    <row r="11" spans="1:30" hidden="1">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2604,9 +2646,9 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2620,34 +2662,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <pane xSplit="16180" topLeftCell="X1" activePane="topRight"/>
-      <selection activeCell="AA2" sqref="AA2"/>
-      <selection pane="topRight" activeCell="AD3" sqref="AD3"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <pane xSplit="26835"/>
+      <selection activeCell="AC20" sqref="AC20"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="14.625" customWidth="1"/>
+    <col min="9" max="9" width="16.875" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="12" max="12" width="11.875" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
     <col min="15" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="7.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.375" customWidth="1"/>
     <col min="21" max="21" width="20" customWidth="1"/>
     <col min="22" max="22" width="13.5" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" customWidth="1"/>
+    <col min="23" max="23" width="15.875" customWidth="1"/>
+    <col min="28" max="28" width="2" customWidth="1"/>
+    <col min="29" max="29" width="30.625" customWidth="1"/>
+    <col min="37" max="37" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16" thickBot="1">
+    <row r="1" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2739,7 +2784,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16" thickTop="1">
+    <row r="2" spans="1:30" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2826,11 +2871,14 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>10MHzStock</v>
       </c>
+      <c r="AC2" t="s">
+        <v>145</v>
+      </c>
       <c r="AD2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2917,11 +2965,14 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHzStock</v>
       </c>
+      <c r="AC3" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="AD3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3005,8 +3056,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHz</v>
       </c>
+      <c r="AC4" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -3090,8 +3144,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHz</v>
       </c>
+      <c r="AC5" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3175,8 +3232,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHz</v>
       </c>
+      <c r="AC6" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -3260,8 +3320,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHz</v>
       </c>
+      <c r="AC7" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3345,8 +3408,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>16MHz</v>
       </c>
+      <c r="AC8" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3433,11 +3499,14 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>20MHzStock</v>
       </c>
+      <c r="AC9" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="AD9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3521,8 +3590,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>20MHz</v>
       </c>
+      <c r="AC10" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3609,11 +3681,14 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHzStock</v>
       </c>
+      <c r="AC11" t="s">
+        <v>145</v>
+      </c>
       <c r="AD11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -3697,8 +3772,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHz</v>
       </c>
+      <c r="AC12" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3782,8 +3860,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHz</v>
       </c>
+      <c r="AC13" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -3867,8 +3948,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHz</v>
       </c>
+      <c r="AC14" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -3952,8 +4036,11 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHz</v>
       </c>
+      <c r="AC15" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -4037,12 +4124,15 @@
         <f>CONCATENATE(Table13[[#This Row],[Frequency]],Table13[[#This Row],[Stock]])</f>
         <v>8MHz</v>
       </c>
+      <c r="AC16" t="s">
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>